<commit_message>
Modificacion en psp'p SC_Lectura
</commit_message>
<xml_diff>
--- a/Documentación/Psp's/Tania/Clase BD_ControlEscolar/ProgramSize.xlsx
+++ b/Documentación/Psp's/Tania/Clase BD_ControlEscolar/ProgramSize.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8760" windowHeight="6750"/>
   </bookViews>
   <sheets>
-    <sheet name="excel" sheetId="1" r:id="rId1"/>
+    <sheet name="excel (1)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="excel" localSheetId="0">excel!$A$1:$D$26</definedName>
+    <definedName name="excel__1" localSheetId="0">'excel (1)'!$A$1:$D$26</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -23,7 +23,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" odcFile="C:\Users\TaniaEsparza\Downloads\excel.iqy" name="excel" type="4" refreshedVersion="5" background="1" saveData="1">
+  <connection id="1" odcFile="C:\Users\TaniaEsparza\AppData\Local\Packages\Microsoft.MicrosoftEdge_8wekyb3d8bbwe\TempState\Downloads\excel (1).iqy" name="excel (1)" type="4" refreshedVersion="5" background="1" saveData="1">
     <webPr consecutive="1" xl2000="1" url="http://localhost:2468/reports/form2html.class?uri=%2FProject%2FCodificacion%2BBD%2BControl%2BEscolar%2FPSP2%2E1%2F%2Fcms%2Fpsp2%2E1%2Fsummary%3Fframe%3Dcontent%26section%3D105&amp;EXPORT=excel" htmlFormat="all"/>
   </connection>
 </connections>
@@ -89,7 +89,7 @@
     <t>Adapted from "PSP Materials," copyright © 2006 Carnegie Mellon University. Used by permission.</t>
   </si>
   <si>
-    <t>Report generated at 8:55 PM on Dec 3, 2018</t>
+    <t>Report generated at 9:51 PM on Dec 6, 2018</t>
   </si>
 </sst>
 </file>
@@ -723,7 +723,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excel" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="excel (1)" preserveFormatting="0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>